<commit_message>
student profile parser improvements
</commit_message>
<xml_diff>
--- a/src/test/resources/parser/master.xlsx
+++ b/src/test/resources/parser/master.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\hneu-personal-account\src\test\resources\parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oleksandrrozdolskyi/Repos/hneu-personal-account/src/test/resources/parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="МАГИСТР" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">МАГИСТР!$A$1:$K$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">МАГИСТР!$16:$16</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">МАГИСТР!$A$1:$K$47</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -88,12 +94,6 @@
   </si>
   <si>
     <t>№</t>
-  </si>
-  <si>
-    <t>МАГІСТЕРСЬКА ПРОГРАМА :</t>
-  </si>
-  <si>
-    <t>СПЕЦІАЛЬНІСТЬ :</t>
   </si>
   <si>
     <t>контактна інформація :</t>
@@ -218,15 +218,21 @@
   <si>
     <t>Дипломний проект</t>
   </si>
+  <si>
+    <t>Спеціалізація:</t>
+  </si>
+  <si>
+    <t>Спеціальність:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +414,13 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -440,11 +453,11 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -453,25 +466,25 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -479,7 +492,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -488,44 +501,44 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,28 +547,28 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -564,86 +577,86 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -968,7 +981,7 @@
         <xdr:cNvPr id="2" name="Группа 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -977,7 +990,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11480205" cy="1357312"/>
+          <a:ext cx="13016111" cy="1349374"/>
           <a:chOff x="10633" y="6"/>
           <a:chExt cx="7649775" cy="854145"/>
         </a:xfrm>
@@ -987,7 +1000,7 @@
           <xdr:cNvPr id="3" name="Рисунок 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1020,7 +1033,7 @@
           <xdr:cNvPr id="4" name="Рисунок 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1053,7 +1066,7 @@
           <xdr:cNvPr id="5" name="Прямоугольник 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1384,7 +1397,7 @@
         <xdr:cNvPr id="6" name="Прямоугольник 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1450,7 +1463,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1744,33 +1757,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="0.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="45.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" style="1" customWidth="1"/>
     <col min="13" max="14" width="30" style="1" customWidth="1"/>
-    <col min="15" max="15" width="39.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="49.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="17.42578125" style="1"/>
+    <col min="15" max="15" width="39.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="49.5" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="17.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="48"/>
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
@@ -1783,9 +1796,9 @@
       <c r="J3" s="48"/>
       <c r="K3" s="48"/>
     </row>
-    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="48" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
@@ -1798,13 +1811,13 @@
       <c r="J4" s="48"/>
       <c r="K4" s="48"/>
     </row>
-    <row r="5" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="43" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
@@ -1812,12 +1825,12 @@
       <c r="G6" s="49"/>
       <c r="H6" s="49"/>
     </row>
-    <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="49"/>
@@ -1825,9 +1838,9 @@
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
     </row>
-    <row r="8" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="51">
         <v>150673</v>
@@ -1838,12 +1851,12 @@
       <c r="G8" s="51"/>
       <c r="H8" s="51"/>
     </row>
-    <row r="9" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="43" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
@@ -1851,9 +1864,9 @@
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
     </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="47">
         <v>2016</v>
@@ -1864,12 +1877,12 @@
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
     </row>
-    <row r="11" spans="1:11" s="42" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" s="42" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="52"/>
       <c r="E11" s="52"/>
@@ -1877,10 +1890,10 @@
       <c r="G11" s="52"/>
       <c r="H11" s="52"/>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41"/>
       <c r="C12" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -1888,13 +1901,13 @@
       <c r="G12" s="50"/>
       <c r="H12" s="50"/>
     </row>
-    <row r="13" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="53" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B13" s="53"/>
       <c r="C13" s="57" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="57"/>
       <c r="E13" s="57"/>
@@ -1905,13 +1918,13 @@
       <c r="J13" s="57"/>
       <c r="K13" s="57"/>
     </row>
-    <row r="14" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B14" s="59"/>
       <c r="C14" s="57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="57"/>
       <c r="E14" s="57"/>
@@ -1922,12 +1935,12 @@
       <c r="J14" s="57"/>
       <c r="K14" s="57"/>
     </row>
-    <row r="15" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="43" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="50"/>
@@ -1935,7 +1948,7 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
     </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="8" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
         <v>19</v>
       </c>
@@ -1949,7 +1962,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="37" t="s">
         <v>19</v>
@@ -1964,10 +1977,10 @@
         <v>16</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="8" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="8" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="11"/>
       <c r="C17" s="10"/>
@@ -1979,7 +1992,7 @@
       <c r="J17" s="10"/>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="54" t="s">
         <v>15</v>
       </c>
@@ -1994,7 +2007,7 @@
       <c r="J18" s="55"/>
       <c r="K18" s="56"/>
     </row>
-    <row r="19" spans="1:16" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="60" t="s">
         <v>14</v>
       </c>
@@ -2010,7 +2023,7 @@
       <c r="J19" s="61"/>
       <c r="K19" s="62"/>
     </row>
-    <row r="20" spans="1:16" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="67" t="s">
         <v>12</v>
       </c>
@@ -2027,25 +2040,25 @@
       <c r="J20" s="65"/>
       <c r="K20" s="66"/>
     </row>
-    <row r="21" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
         <v>1</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="24">
         <v>5</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E21" s="22"/>
       <c r="G21" s="23">
         <v>1</v>
       </c>
       <c r="H21" s="36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I21" s="24">
         <v>4</v>
@@ -2055,12 +2068,12 @@
       </c>
       <c r="K21" s="31"/>
     </row>
-    <row r="22" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="26">
         <v>2</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="24">
         <v>5</v>
@@ -2073,73 +2086,73 @@
         <v>2</v>
       </c>
       <c r="H22" s="36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I22" s="24">
         <v>5</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
         <v>3</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="24">
         <v>5</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E23" s="22"/>
       <c r="G23" s="23">
         <v>3</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I23" s="24">
         <v>5</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K23" s="31"/>
     </row>
-    <row r="24" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="26">
         <v>4</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="24">
         <v>5</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E24" s="22"/>
       <c r="G24" s="23">
         <v>4</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I24" s="24">
         <v>5</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K24" s="31"/>
     </row>
-    <row r="25" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="46">
         <f>IF(B25=0,0,A24+1)</f>
         <v>0</v>
@@ -2151,17 +2164,17 @@
         <v>5</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I25" s="24">
         <v>1</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K25" s="31"/>
     </row>
-    <row r="26" spans="1:16" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="67" t="s">
         <v>11</v>
       </c>
@@ -2178,7 +2191,7 @@
       <c r="J26" s="64"/>
       <c r="K26" s="68"/>
     </row>
-    <row r="27" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <f>IF(B27=0,0,MAX(A22:A25)+1)</f>
         <v>0</v>
@@ -2216,7 +2229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
         <f>IF(B28=0,0,A27+1)</f>
         <v>0</v>
@@ -2254,7 +2267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="8" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="8" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <f>IF(B29=0,0,#REF!+1)</f>
         <v>0</v>
@@ -2269,7 +2282,7 @@
       <c r="I29" s="11"/>
       <c r="K29" s="18"/>
     </row>
-    <row r="30" spans="1:16" s="12" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" s="12" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="16" t="str">
         <f>CONCATENATE("ВСЬОГО ЗА ",A19)</f>
@@ -2294,7 +2307,7 @@
       <c r="J30" s="14"/>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:16" s="8" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" s="8" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="11"/>
       <c r="C31" s="10"/>
@@ -2306,7 +2319,7 @@
       <c r="J31" s="10"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="54" t="s">
         <v>3</v>
       </c>
@@ -2321,7 +2334,7 @@
       <c r="J32" s="55"/>
       <c r="K32" s="56"/>
     </row>
-    <row r="33" spans="1:11" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="60" t="s">
         <v>2</v>
       </c>
@@ -2335,7 +2348,7 @@
       <c r="J33" s="61"/>
       <c r="K33" s="62"/>
     </row>
-    <row r="34" spans="1:11" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="63" t="s">
         <v>1</v>
       </c>
@@ -2350,79 +2363,79 @@
       <c r="J34" s="65"/>
       <c r="K34" s="66"/>
     </row>
-    <row r="35" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
         <v>1</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="24">
         <v>3</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E35" s="22"/>
       <c r="H35" s="19"/>
       <c r="I35" s="11"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="26">
         <v>2</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="24">
         <v>8</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E36" s="22"/>
       <c r="H36" s="19"/>
       <c r="I36" s="11"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
         <v>3</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C37" s="24">
         <v>4</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E37" s="22"/>
       <c r="H37" s="19"/>
       <c r="I37" s="11"/>
       <c r="K37" s="21"/>
     </row>
-    <row r="38" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="26">
         <v>4</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C38" s="24">
         <v>15</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E38" s="22"/>
       <c r="H38" s="19"/>
       <c r="I38" s="11"/>
       <c r="K38" s="21"/>
     </row>
-    <row r="39" spans="1:11" s="8" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="8" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20">
         <f>IF(B39=0,0,#REF!+1)</f>
         <v>0</v>
@@ -2433,7 +2446,7 @@
       <c r="I39" s="11"/>
       <c r="K39" s="18"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" s="12" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="16" t="str">
         <f>CONCATENATE("ВСЬОГО ЗА ",A33)</f>
@@ -2452,7 +2465,7 @@
       <c r="J40" s="14"/>
       <c r="K40" s="13"/>
     </row>
-    <row r="41" spans="1:11" s="8" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="8" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="11"/>
       <c r="C41" s="10"/>
@@ -2464,12 +2477,12 @@
       <c r="J41" s="10"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7">
         <f ca="1">TODAY(  )</f>
-        <v>42813</v>
+        <v>42934</v>
       </c>
       <c r="C44" s="58" t="str">
         <f>CONCATENATE("_________________________",LEFT(C7,1)&amp;". ",C6)</f>
@@ -2481,27 +2494,27 @@
       <c r="G44" s="58"/>
       <c r="H44" s="58"/>
     </row>
-    <row r="45" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:11" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
         <v>0</v>
       </c>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:11" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="str">
         <f>CONCATENATE(C9," ___________________________________________")</f>
         <v>Економічної інформатики ___________________________________________</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.2">
       <c r="G48" s="4"/>
     </row>
   </sheetData>
@@ -2534,6 +2547,7 @@
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C8:H8"/>
   </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="D21:D25">
     <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"Екзамен"</formula>

</xml_diff>

<commit_message>
move pages to thyme leaf
</commit_message>
<xml_diff>
--- a/src/test/resources/parser/master.xlsx
+++ b/src/test/resources/parser/master.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">МАГИСТР!$A$1:$K$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">МАГИСТР!$16:$16</definedName>
   </definedNames>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>Декан факультету</t>
   </si>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">Сучасна теорія управління </t>
   </si>
   <si>
-    <t>122 КОМП'ЮТЕРНІ НАУКИ ТА ІНФОРМАЦІЙНІ ТЕХНОЛОГІЇ</t>
-  </si>
-  <si>
     <t>Оцінка</t>
   </si>
   <si>
@@ -224,6 +221,12 @@
   <si>
     <t>Спеціальність:</t>
   </si>
+  <si>
+    <t>Комп'ютерні науки</t>
+  </si>
+  <si>
+    <t>ДИПЛОМНА РОБОТА</t>
+  </si>
 </sst>
 </file>
 
@@ -232,7 +235,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +424,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -661,9 +673,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -805,6 +818,60 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -814,67 +881,14 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -981,7 +995,7 @@
         <xdr:cNvPr id="2" name="Группа 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1000,7 +1014,7 @@
           <xdr:cNvPr id="3" name="Рисунок 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1033,7 +1047,7 @@
           <xdr:cNvPr id="4" name="Рисунок 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1066,7 +1080,7 @@
           <xdr:cNvPr id="5" name="Прямоугольник 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1397,7 +1411,7 @@
         <xdr:cNvPr id="6" name="Прямоугольник 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1463,7 +1477,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1757,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:H12"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1784,166 +1798,166 @@
     <row r="1" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
     </row>
     <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
     </row>
     <row r="5" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="C6" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
     </row>
     <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
+      <c r="C7" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
     </row>
     <row r="8" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="68">
         <v>150673</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
     </row>
     <row r="9" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="65">
         <v>2016</v>
       </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
     </row>
     <row r="11" spans="1:11" s="42" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
+      <c r="C11" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41"/>
-      <c r="C12" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
+      <c r="C12" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
     </row>
     <row r="13" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
     </row>
     <row r="14" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
+      <c r="A14" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
     </row>
     <row r="15" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
+      <c r="C15" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="40"/>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
@@ -1962,7 +1976,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="37" t="s">
         <v>19</v>
@@ -1977,7 +1991,7 @@
         <v>16</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1993,52 +2007,52 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="52"/>
     </row>
     <row r="19" spans="1:16" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="G19" s="61" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="G19" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="62"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="55"/>
     </row>
     <row r="20" spans="1:16" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
       <c r="F20" s="27"/>
-      <c r="G20" s="65" t="s">
+      <c r="G20" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="66"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
@@ -2086,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I22" s="24">
         <v>5</v>
@@ -2101,7 +2115,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="24">
         <v>5</v>
@@ -2114,7 +2128,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I23" s="24">
         <v>5</v>
@@ -2129,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="24">
         <v>5</v>
@@ -2142,7 +2156,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I24" s="24">
         <v>5</v>
@@ -2175,21 +2189,21 @@
       <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:16" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="64" t="s">
+      <c r="G26" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="65"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="68"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="62"/>
     </row>
     <row r="27" spans="1:16" s="8" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
@@ -2320,48 +2334,48 @@
       <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="56"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="52"/>
     </row>
     <row r="33" spans="1:11" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="62"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="55"/>
     </row>
     <row r="34" spans="1:11" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="63" t="s">
+      <c r="A34" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="64"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
       <c r="F34" s="27"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="66"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="59"/>
     </row>
     <row r="35" spans="1:11" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
@@ -2386,7 +2400,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="24">
         <v>8</v>
@@ -2422,13 +2436,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C38" s="24">
         <v>15</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E38" s="22"/>
       <c r="H38" s="19"/>
@@ -2482,17 +2496,17 @@
     <row r="44" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7">
         <f ca="1">TODAY(  )</f>
-        <v>42934</v>
-      </c>
-      <c r="C44" s="58" t="str">
+        <v>42981</v>
+      </c>
+      <c r="C44" s="47" t="str">
         <f>CONCATENATE("_________________________",LEFT(C7,1)&amp;". ",C6)</f>
         <v>_________________________О. Роздольський</v>
       </c>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
     </row>
     <row r="45" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
@@ -2511,7 +2525,7 @@
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.2">
@@ -2519,6 +2533,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="C13:K13"/>
     <mergeCell ref="C44:H44"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:K14"/>
@@ -2534,18 +2560,6 @@
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="G26:K26"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C8:H8"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="D21:D25">

</xml_diff>